<commit_message>
Update plan and design
</commit_message>
<xml_diff>
--- a/W6Project/Plan/Plan.xlsx
+++ b/W6Project/Plan/Plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="57">
   <si>
     <t>ERD Design</t>
   </si>
@@ -557,7 +557,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -886,84 +886,112 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G13" t="s">
+      <c r="F13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="5" t="s">
         <v>35</v>
       </c>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="6">
         <v>2</v>
       </c>
-      <c r="E14" t="s">
+      <c r="D14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G14" t="s">
+      <c r="F14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6">
         <v>2</v>
       </c>
-      <c r="E15" t="s">
+      <c r="D15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G15" t="s">
+      <c r="F15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="B16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="6">
         <v>2</v>
       </c>
-      <c r="E16" t="s">
+      <c r="D16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G16" t="s">
+      <c r="F16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="45">
       <c r="A17" t="s">

</xml_diff>